<commit_message>
Test mit allen Versuchen
</commit_message>
<xml_diff>
--- a/Verwendete_Ports.xlsx
+++ b/Verwendete_Ports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxin\Desktop\HackerLab\VirtualHackerLab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350dbd18d7049cf/Master/Jahresprojekt/HackerLab/HackerLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFF24D7E-4440-42C7-9684-5D429A13742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{FFF24D7E-4440-42C7-9684-5D429A13742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5259F2CC-F96A-4431-9844-A257DC844B27}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{12661B78-1DDC-490F-AB02-E6DDD402F114}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12661B78-1DDC-490F-AB02-E6DDD402F114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Service-Typ</t>
   </si>
@@ -80,9 +80,6 @@
     <t>1389:1389</t>
   </si>
   <si>
-    <t>1390:1390</t>
-  </si>
-  <si>
     <t>8082:8082</t>
   </si>
   <si>
@@ -99,6 +96,18 @@
   </si>
   <si>
     <t>3306:3306</t>
+  </si>
+  <si>
+    <t>Webshell</t>
+  </si>
+  <si>
+    <t>3307:3307</t>
+  </si>
+  <si>
+    <t>8082:82</t>
+  </si>
+  <si>
+    <t>10389:10390</t>
   </si>
 </sst>
 </file>
@@ -142,17 +151,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,7 +177,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -464,32 +473,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64292C1-8DB5-4158-8543-D3DDD128B52B}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -499,8 +508,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -508,8 +517,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -517,8 +526,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -528,8 +537,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -537,58 +546,82 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="4">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2">
         <v>0.93194444444444446</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Neue Version Log4Shell & Port Änderungen
</commit_message>
<xml_diff>
--- a/Verwendete_Ports.xlsx
+++ b/Verwendete_Ports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350dbd18d7049cf/Master/Jahresprojekt/HackerLab/HackerLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{FFF24D7E-4440-42C7-9684-5D429A13742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5259F2CC-F96A-4431-9844-A257DC844B27}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{FFF24D7E-4440-42C7-9684-5D429A13742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{514C5A51-8ECF-4E8E-84EA-B7476A2DEE84}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12661B78-1DDC-490F-AB02-E6DDD402F114}"/>
   </bookViews>
@@ -104,10 +104,10 @@
     <t>3307:3307</t>
   </si>
   <si>
-    <t>8082:82</t>
-  </si>
-  <si>
     <t>10389:10390</t>
+  </si>
+  <si>
+    <t>8090:90</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed pw crack db port
</commit_message>
<xml_diff>
--- a/Verwendete_Ports.xlsx
+++ b/Verwendete_Ports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350dbd18d7049cf/Master/Jahresprojekt/HackerLab/HackerLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{FFF24D7E-4440-42C7-9684-5D429A13742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{514C5A51-8ECF-4E8E-84EA-B7476A2DEE84}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{FFF24D7E-4440-42C7-9684-5D429A13742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AA61478-E721-4DDB-BB51-8CE83F886079}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12661B78-1DDC-490F-AB02-E6DDD402F114}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>VirtualHackerLab Website</t>
   </si>
   <si>
-    <t>1201:1201</t>
-  </si>
-  <si>
     <t>Log4Shell_Gepatched</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>8090:90</t>
+  </si>
+  <si>
+    <t>3307:3306</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,64 +523,64 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>80</v>
@@ -589,7 +589,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>0.93194444444444446</v>
@@ -597,13 +597,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>